<commit_message>
Add tests, coverage, on-demand workflow, retries, and summary for failed rows
</commit_message>
<xml_diff>
--- a/input/repos_example.xlsx
+++ b/input/repos_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a7119f9a48e1aa7/Cursor/JiraFlowEval/repo_evaluator/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a7119f9a48e1aa7/Cursor/JiraFlowEval/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85BA63B2-6EE4-4BBA-BBFF-C656071E2B55}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7F930D-5CF5-4FB0-B258-347AB0CE0601}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,15 +412,15 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -442,7 +442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update input repo list (repos_example.xlsx)
</commit_message>
<xml_diff>
--- a/input/repos_example.xlsx
+++ b/input/repos_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a7119f9a48e1aa7/Cursor/JiraFlowEval/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E7F930D-5CF5-4FB0-B258-347AB0CE0601}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2B59D2BFD380D14AEF0D7B32443088B35299F3AE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D29E23BA-8C2D-4411-B6E4-5A9835F61432}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>https://github.com/example/data-pipeline-1</t>
-  </si>
-  <si>
-    <t>Alice</t>
-  </si>
-  <si>
-    <t>alice@example.com</t>
-  </si>
-  <si>
     <t>https://github.com/example/data-pipeline-2</t>
   </si>
   <si>
@@ -47,13 +38,22 @@
   </si>
   <si>
     <t>bob@example.com</t>
+  </si>
+  <si>
+    <t>https://github.com/danielhantunes/JiraFlow</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>danielh.engenhariadesistemas@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +65,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,16 +107,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,12 +423,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -432,28 +444,32 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3E97C23D-40D0-4620-A5FF-AEBB0472D40D}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00337001-EFDD-43D3-963F-C9BD1021468D}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>